<commit_message>
valorizzata la colonna O del report-checklist.xlsx
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111METEDA00000/METEDA_S.r.l/MetaClinic/10/report-checklist.xlsx
+++ b/GATEWAY/S1#111METEDA00000/METEDA_S.r.l/MetaClinic/10/report-checklist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_documentazione\CDA2\accreditamento\it-fse-accreditamento-main\GATEWAY\S1#111METEDA00000\METEDA_S.r.l\MetaClinic\10\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ministero\it-fse-accreditamento\GATEWAY\S1#111METEDA00000\METEDA_S.r.l\MetaClinic\10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7958C5A-0F08-427D-A324-C1CE74F6E7AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D5C135-188D-436E-94A1-7D06B441DD09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2181" uniqueCount="896">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2211" uniqueCount="897">
   <si>
     <t>NOME FORNITORE:</t>
   </si>
@@ -4607,6 +4607,9 @@
   </si>
   <si>
     <t>L'applicativo non gestisce la parte codificata della section Situazione_Clinica e delle sue sottosezioni</t>
+  </si>
+  <si>
+    <t>potrebbe essere ricondotta ad una gestione in back office qualora l'utente al verificarsi dell'errore decide di non proseguire e contatta il supporto tecnico qualora non sia in grado di risolvere il problema in autonomia.</t>
   </si>
 </sst>
 </file>
@@ -5269,10 +5272,10 @@
   <dimension ref="A1:T992"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="F348" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="O348" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="J379" sqref="J379"/>
+      <selection pane="bottomRight" activeCell="S352" sqref="S352"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -16689,13 +16692,17 @@
       <c r="N334" s="17" t="s">
         <v>842</v>
       </c>
-      <c r="O334" s="17"/>
+      <c r="O334" s="17" t="s">
+        <v>807</v>
+      </c>
       <c r="P334" s="17" t="s">
         <v>826</v>
       </c>
       <c r="Q334" s="17"/>
       <c r="R334" s="18"/>
-      <c r="S334" s="19"/>
+      <c r="S334" s="19" t="s">
+        <v>896</v>
+      </c>
       <c r="T334" s="20" t="s">
         <v>29</v>
       </c>
@@ -16741,13 +16748,17 @@
       <c r="N335" s="17" t="s">
         <v>827</v>
       </c>
-      <c r="O335" s="17"/>
+      <c r="O335" s="17" t="s">
+        <v>807</v>
+      </c>
       <c r="P335" s="17" t="s">
         <v>826</v>
       </c>
       <c r="Q335" s="17"/>
       <c r="R335" s="18"/>
-      <c r="S335" s="19"/>
+      <c r="S335" s="19" t="s">
+        <v>896</v>
+      </c>
       <c r="T335" s="20" t="s">
         <v>29</v>
       </c>
@@ -16793,13 +16804,17 @@
       <c r="N336" s="17" t="s">
         <v>828</v>
       </c>
-      <c r="O336" s="17"/>
+      <c r="O336" s="17" t="s">
+        <v>807</v>
+      </c>
       <c r="P336" s="17" t="s">
         <v>826</v>
       </c>
       <c r="Q336" s="17"/>
       <c r="R336" s="18"/>
-      <c r="S336" s="19"/>
+      <c r="S336" s="19" t="s">
+        <v>896</v>
+      </c>
       <c r="T336" s="20" t="s">
         <v>29</v>
       </c>
@@ -16845,13 +16860,17 @@
       <c r="N337" s="17" t="s">
         <v>829</v>
       </c>
-      <c r="O337" s="17"/>
+      <c r="O337" s="17" t="s">
+        <v>807</v>
+      </c>
       <c r="P337" s="17" t="s">
         <v>826</v>
       </c>
       <c r="Q337" s="17"/>
       <c r="R337" s="18"/>
-      <c r="S337" s="19"/>
+      <c r="S337" s="19" t="s">
+        <v>896</v>
+      </c>
       <c r="T337" s="20" t="s">
         <v>29</v>
       </c>
@@ -16897,13 +16916,17 @@
       <c r="N338" s="17" t="s">
         <v>830</v>
       </c>
-      <c r="O338" s="17"/>
+      <c r="O338" s="17" t="s">
+        <v>807</v>
+      </c>
       <c r="P338" s="17" t="s">
         <v>826</v>
       </c>
       <c r="Q338" s="17"/>
       <c r="R338" s="18"/>
-      <c r="S338" s="19"/>
+      <c r="S338" s="19" t="s">
+        <v>896</v>
+      </c>
       <c r="T338" s="20" t="s">
         <v>29</v>
       </c>
@@ -16949,13 +16972,17 @@
       <c r="N339" s="17" t="s">
         <v>858</v>
       </c>
-      <c r="O339" s="17"/>
+      <c r="O339" s="17" t="s">
+        <v>807</v>
+      </c>
       <c r="P339" s="17" t="s">
         <v>826</v>
       </c>
       <c r="Q339" s="17"/>
       <c r="R339" s="18"/>
-      <c r="S339" s="19"/>
+      <c r="S339" s="19" t="s">
+        <v>896</v>
+      </c>
       <c r="T339" s="20" t="s">
         <v>29</v>
       </c>
@@ -17001,13 +17028,17 @@
       <c r="N340" s="17" t="s">
         <v>831</v>
       </c>
-      <c r="O340" s="17"/>
+      <c r="O340" s="17" t="s">
+        <v>807</v>
+      </c>
       <c r="P340" s="17" t="s">
         <v>826</v>
       </c>
       <c r="Q340" s="17"/>
       <c r="R340" s="18"/>
-      <c r="S340" s="19"/>
+      <c r="S340" s="19" t="s">
+        <v>896</v>
+      </c>
       <c r="T340" s="20" t="s">
         <v>29</v>
       </c>
@@ -17053,13 +17084,17 @@
       <c r="N341" s="17" t="s">
         <v>865</v>
       </c>
-      <c r="O341" s="17"/>
+      <c r="O341" s="17" t="s">
+        <v>807</v>
+      </c>
       <c r="P341" s="17" t="s">
         <v>826</v>
       </c>
       <c r="Q341" s="17"/>
       <c r="R341" s="18"/>
-      <c r="S341" s="19"/>
+      <c r="S341" s="19" t="s">
+        <v>896</v>
+      </c>
       <c r="T341" s="20" t="s">
         <v>29</v>
       </c>
@@ -17105,13 +17140,17 @@
       <c r="N342" s="17" t="s">
         <v>869</v>
       </c>
-      <c r="O342" s="17"/>
+      <c r="O342" s="17" t="s">
+        <v>807</v>
+      </c>
       <c r="P342" s="17" t="s">
         <v>826</v>
       </c>
       <c r="Q342" s="17"/>
       <c r="R342" s="18"/>
-      <c r="S342" s="19"/>
+      <c r="S342" s="19" t="s">
+        <v>896</v>
+      </c>
       <c r="T342" s="20" t="s">
         <v>29</v>
       </c>
@@ -17157,13 +17196,17 @@
       <c r="N343" s="17" t="s">
         <v>873</v>
       </c>
-      <c r="O343" s="17"/>
+      <c r="O343" s="17" t="s">
+        <v>807</v>
+      </c>
       <c r="P343" s="17" t="s">
         <v>826</v>
       </c>
       <c r="Q343" s="17"/>
       <c r="R343" s="18"/>
-      <c r="S343" s="19"/>
+      <c r="S343" s="19" t="s">
+        <v>896</v>
+      </c>
       <c r="T343" s="20" t="s">
         <v>29</v>
       </c>
@@ -17209,13 +17252,17 @@
       <c r="N344" s="17" t="s">
         <v>877</v>
       </c>
-      <c r="O344" s="17"/>
+      <c r="O344" s="17" t="s">
+        <v>807</v>
+      </c>
       <c r="P344" s="17" t="s">
         <v>826</v>
       </c>
       <c r="Q344" s="17"/>
       <c r="R344" s="18"/>
-      <c r="S344" s="19"/>
+      <c r="S344" s="19" t="s">
+        <v>896</v>
+      </c>
       <c r="T344" s="20" t="s">
         <v>29</v>
       </c>
@@ -17261,13 +17308,17 @@
       <c r="N345" s="17" t="s">
         <v>881</v>
       </c>
-      <c r="O345" s="17"/>
+      <c r="O345" s="17" t="s">
+        <v>807</v>
+      </c>
       <c r="P345" s="17" t="s">
         <v>826</v>
       </c>
       <c r="Q345" s="17"/>
       <c r="R345" s="18"/>
-      <c r="S345" s="19"/>
+      <c r="S345" s="19" t="s">
+        <v>896</v>
+      </c>
       <c r="T345" s="20" t="s">
         <v>29</v>
       </c>
@@ -17313,13 +17364,17 @@
       <c r="N346" s="17" t="s">
         <v>885</v>
       </c>
-      <c r="O346" s="17"/>
+      <c r="O346" s="17" t="s">
+        <v>807</v>
+      </c>
       <c r="P346" s="17" t="s">
         <v>826</v>
       </c>
       <c r="Q346" s="17"/>
       <c r="R346" s="18"/>
-      <c r="S346" s="19"/>
+      <c r="S346" s="19" t="s">
+        <v>896</v>
+      </c>
       <c r="T346" s="20" t="s">
         <v>29</v>
       </c>
@@ -17525,13 +17580,17 @@
       <c r="N351" s="17" t="s">
         <v>889</v>
       </c>
-      <c r="O351" s="17"/>
+      <c r="O351" s="17" t="s">
+        <v>807</v>
+      </c>
       <c r="P351" s="17" t="s">
         <v>826</v>
       </c>
       <c r="Q351" s="17"/>
       <c r="R351" s="18"/>
-      <c r="S351" s="19"/>
+      <c r="S351" s="19" t="s">
+        <v>896</v>
+      </c>
       <c r="T351" s="20" t="s">
         <v>29</v>
       </c>
@@ -17577,13 +17636,17 @@
       <c r="N352" s="17" t="s">
         <v>893</v>
       </c>
-      <c r="O352" s="17"/>
+      <c r="O352" s="17" t="s">
+        <v>807</v>
+      </c>
       <c r="P352" s="17" t="s">
         <v>826</v>
       </c>
       <c r="Q352" s="17"/>
       <c r="R352" s="18"/>
-      <c r="S352" s="19"/>
+      <c r="S352" s="19" t="s">
+        <v>896</v>
+      </c>
       <c r="T352" s="20" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
corretto il caso di test 147
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111METEDA00000/METEDA_S.r.l/MetaClinic/10/report-checklist.xlsx
+++ b/GATEWAY/S1#111METEDA00000/METEDA_S.r.l/MetaClinic/10/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ministero\it-fse-accreditamento\GATEWAY\S1#111METEDA00000\METEDA_S.r.l\MetaClinic\10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D5C135-188D-436E-94A1-7D06B441DD09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DCC17AF-983F-4D59-91EA-41019A0932B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4399,15 +4399,6 @@
     <t>L'applicativo non gestisce tutte le sezioni opzionali previste dal caso di test</t>
   </si>
   <si>
-    <t>2023-05-17T09:51:54Z</t>
-  </si>
-  <si>
-    <t>154d193332cb2ff0</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.63e6ec4c76adbacd330764827d38de6d8326e9a3c066c43551ace482608d95e1.e216c5a9a7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>2023-05-17T10:10:40Z</t>
   </si>
   <si>
@@ -4610,6 +4601,15 @@
   </si>
   <si>
     <t>potrebbe essere ricondotta ad una gestione in back office qualora l'utente al verificarsi dell'errore decide di non proseguire e contatta il supporto tecnico qualora non sia in grado di risolvere il problema in autonomia.</t>
+  </si>
+  <si>
+    <t>fc96c44d466fcf92</t>
+  </si>
+  <si>
+    <t>2023-05-24T14:20:57Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.eece9f1dfc8c6fd7196add6a0fe7144452444480534dee78808cb502127a86d4.2d7ca8be18^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -5272,10 +5272,10 @@
   <dimension ref="A1:T992"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="O348" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="F231" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="S352" sqref="S352"/>
+      <selection pane="bottomRight" activeCell="I330" sqref="I330"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -16504,16 +16504,16 @@
         <v>666</v>
       </c>
       <c r="F330" s="15">
-        <v>45063</v>
+        <v>45070</v>
       </c>
       <c r="G330" s="16" t="s">
-        <v>836</v>
+        <v>895</v>
       </c>
       <c r="H330" s="16" t="s">
-        <v>837</v>
+        <v>894</v>
       </c>
       <c r="I330" s="16" t="s">
-        <v>838</v>
+        <v>896</v>
       </c>
       <c r="J330" s="17" t="s">
         <v>467</v>
@@ -16671,13 +16671,13 @@
         <v>45063</v>
       </c>
       <c r="G334" s="16" t="s">
-        <v>839</v>
+        <v>836</v>
       </c>
       <c r="H334" s="16" t="s">
-        <v>840</v>
+        <v>837</v>
       </c>
       <c r="I334" s="16" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="J334" s="17" t="s">
         <v>467</v>
@@ -16690,7 +16690,7 @@
         <v>467</v>
       </c>
       <c r="N334" s="17" t="s">
-        <v>842</v>
+        <v>839</v>
       </c>
       <c r="O334" s="17" t="s">
         <v>807</v>
@@ -16701,7 +16701,7 @@
       <c r="Q334" s="17"/>
       <c r="R334" s="18"/>
       <c r="S334" s="19" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="T334" s="20" t="s">
         <v>29</v>
@@ -16727,13 +16727,13 @@
         <v>45063</v>
       </c>
       <c r="G335" s="16" t="s">
-        <v>843</v>
+        <v>840</v>
       </c>
       <c r="H335" s="16" t="s">
-        <v>844</v>
+        <v>841</v>
       </c>
       <c r="I335" s="16" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
       <c r="J335" s="17" t="s">
         <v>467</v>
@@ -16757,7 +16757,7 @@
       <c r="Q335" s="17"/>
       <c r="R335" s="18"/>
       <c r="S335" s="19" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="T335" s="20" t="s">
         <v>29</v>
@@ -16783,13 +16783,13 @@
         <v>45063</v>
       </c>
       <c r="G336" s="16" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="H336" s="16" t="s">
-        <v>847</v>
+        <v>844</v>
       </c>
       <c r="I336" s="16" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="J336" s="17" t="s">
         <v>467</v>
@@ -16813,7 +16813,7 @@
       <c r="Q336" s="17"/>
       <c r="R336" s="18"/>
       <c r="S336" s="19" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="T336" s="20" t="s">
         <v>29</v>
@@ -16839,13 +16839,13 @@
         <v>45063</v>
       </c>
       <c r="G337" s="16" t="s">
-        <v>849</v>
+        <v>846</v>
       </c>
       <c r="H337" s="28" t="s">
-        <v>850</v>
+        <v>847</v>
       </c>
       <c r="I337" s="16" t="s">
-        <v>851</v>
+        <v>848</v>
       </c>
       <c r="J337" s="17" t="s">
         <v>467</v>
@@ -16869,7 +16869,7 @@
       <c r="Q337" s="17"/>
       <c r="R337" s="18"/>
       <c r="S337" s="19" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="T337" s="20" t="s">
         <v>29</v>
@@ -16895,13 +16895,13 @@
         <v>45063</v>
       </c>
       <c r="G338" s="16" t="s">
-        <v>852</v>
+        <v>849</v>
       </c>
       <c r="H338" s="16" t="s">
-        <v>853</v>
+        <v>850</v>
       </c>
       <c r="I338" s="16" t="s">
-        <v>854</v>
+        <v>851</v>
       </c>
       <c r="J338" s="17" t="s">
         <v>467</v>
@@ -16925,7 +16925,7 @@
       <c r="Q338" s="17"/>
       <c r="R338" s="18"/>
       <c r="S338" s="19" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="T338" s="20" t="s">
         <v>29</v>
@@ -16951,13 +16951,13 @@
         <v>45063</v>
       </c>
       <c r="G339" s="16" t="s">
-        <v>855</v>
+        <v>852</v>
       </c>
       <c r="H339" s="16" t="s">
-        <v>856</v>
+        <v>853</v>
       </c>
       <c r="I339" s="16" t="s">
-        <v>857</v>
+        <v>854</v>
       </c>
       <c r="J339" s="17" t="s">
         <v>467</v>
@@ -16970,7 +16970,7 @@
         <v>467</v>
       </c>
       <c r="N339" s="17" t="s">
-        <v>858</v>
+        <v>855</v>
       </c>
       <c r="O339" s="17" t="s">
         <v>807</v>
@@ -16981,7 +16981,7 @@
       <c r="Q339" s="17"/>
       <c r="R339" s="18"/>
       <c r="S339" s="19" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="T339" s="20" t="s">
         <v>29</v>
@@ -17007,13 +17007,13 @@
         <v>45063</v>
       </c>
       <c r="G340" s="16" t="s">
-        <v>859</v>
+        <v>856</v>
       </c>
       <c r="H340" s="16" t="s">
-        <v>860</v>
+        <v>857</v>
       </c>
       <c r="I340" s="16" t="s">
-        <v>861</v>
+        <v>858</v>
       </c>
       <c r="J340" s="17" t="s">
         <v>467</v>
@@ -17037,7 +17037,7 @@
       <c r="Q340" s="17"/>
       <c r="R340" s="18"/>
       <c r="S340" s="19" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="T340" s="20" t="s">
         <v>29</v>
@@ -17063,13 +17063,13 @@
         <v>45063</v>
       </c>
       <c r="G341" s="16" t="s">
-        <v>862</v>
+        <v>859</v>
       </c>
       <c r="H341" s="16" t="s">
-        <v>863</v>
+        <v>860</v>
       </c>
       <c r="I341" s="16" t="s">
-        <v>864</v>
+        <v>861</v>
       </c>
       <c r="J341" s="17" t="s">
         <v>467</v>
@@ -17082,7 +17082,7 @@
         <v>467</v>
       </c>
       <c r="N341" s="17" t="s">
-        <v>865</v>
+        <v>862</v>
       </c>
       <c r="O341" s="17" t="s">
         <v>807</v>
@@ -17093,7 +17093,7 @@
       <c r="Q341" s="17"/>
       <c r="R341" s="18"/>
       <c r="S341" s="19" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="T341" s="20" t="s">
         <v>29</v>
@@ -17119,13 +17119,13 @@
         <v>45063</v>
       </c>
       <c r="G342" s="16" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="H342" s="16" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="I342" s="16" t="s">
-        <v>868</v>
+        <v>865</v>
       </c>
       <c r="J342" s="17" t="s">
         <v>467</v>
@@ -17138,7 +17138,7 @@
         <v>467</v>
       </c>
       <c r="N342" s="17" t="s">
-        <v>869</v>
+        <v>866</v>
       </c>
       <c r="O342" s="17" t="s">
         <v>807</v>
@@ -17149,7 +17149,7 @@
       <c r="Q342" s="17"/>
       <c r="R342" s="18"/>
       <c r="S342" s="19" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="T342" s="20" t="s">
         <v>29</v>
@@ -17175,13 +17175,13 @@
         <v>45063</v>
       </c>
       <c r="G343" s="16" t="s">
-        <v>870</v>
+        <v>867</v>
       </c>
       <c r="H343" s="16" t="s">
-        <v>871</v>
+        <v>868</v>
       </c>
       <c r="I343" s="16" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
       <c r="J343" s="17" t="s">
         <v>467</v>
@@ -17194,7 +17194,7 @@
         <v>467</v>
       </c>
       <c r="N343" s="17" t="s">
-        <v>873</v>
+        <v>870</v>
       </c>
       <c r="O343" s="17" t="s">
         <v>807</v>
@@ -17205,7 +17205,7 @@
       <c r="Q343" s="17"/>
       <c r="R343" s="18"/>
       <c r="S343" s="19" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="T343" s="20" t="s">
         <v>29</v>
@@ -17231,13 +17231,13 @@
         <v>45063</v>
       </c>
       <c r="G344" s="16" t="s">
-        <v>874</v>
+        <v>871</v>
       </c>
       <c r="H344" s="16" t="s">
-        <v>875</v>
+        <v>872</v>
       </c>
       <c r="I344" s="16" t="s">
-        <v>876</v>
+        <v>873</v>
       </c>
       <c r="J344" s="17" t="s">
         <v>467</v>
@@ -17250,7 +17250,7 @@
         <v>467</v>
       </c>
       <c r="N344" s="17" t="s">
-        <v>877</v>
+        <v>874</v>
       </c>
       <c r="O344" s="17" t="s">
         <v>807</v>
@@ -17261,7 +17261,7 @@
       <c r="Q344" s="17"/>
       <c r="R344" s="18"/>
       <c r="S344" s="19" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="T344" s="20" t="s">
         <v>29</v>
@@ -17287,13 +17287,13 @@
         <v>45063</v>
       </c>
       <c r="G345" s="16" t="s">
-        <v>878</v>
+        <v>875</v>
       </c>
       <c r="H345" s="16" t="s">
-        <v>879</v>
+        <v>876</v>
       </c>
       <c r="I345" s="16" t="s">
-        <v>880</v>
+        <v>877</v>
       </c>
       <c r="J345" s="17" t="s">
         <v>467</v>
@@ -17306,7 +17306,7 @@
         <v>467</v>
       </c>
       <c r="N345" s="17" t="s">
-        <v>881</v>
+        <v>878</v>
       </c>
       <c r="O345" s="17" t="s">
         <v>807</v>
@@ -17317,7 +17317,7 @@
       <c r="Q345" s="17"/>
       <c r="R345" s="18"/>
       <c r="S345" s="19" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="T345" s="20" t="s">
         <v>29</v>
@@ -17343,13 +17343,13 @@
         <v>45063</v>
       </c>
       <c r="G346" s="16" t="s">
-        <v>882</v>
+        <v>879</v>
       </c>
       <c r="H346" s="16" t="s">
-        <v>883</v>
+        <v>880</v>
       </c>
       <c r="I346" s="16" t="s">
-        <v>884</v>
+        <v>881</v>
       </c>
       <c r="J346" s="17" t="s">
         <v>467</v>
@@ -17362,7 +17362,7 @@
         <v>467</v>
       </c>
       <c r="N346" s="17" t="s">
-        <v>885</v>
+        <v>882</v>
       </c>
       <c r="O346" s="17" t="s">
         <v>807</v>
@@ -17373,7 +17373,7 @@
       <c r="Q346" s="17"/>
       <c r="R346" s="18"/>
       <c r="S346" s="19" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="T346" s="20" t="s">
         <v>29</v>
@@ -17403,7 +17403,7 @@
         <v>807</v>
       </c>
       <c r="K347" s="17" t="s">
-        <v>894</v>
+        <v>891</v>
       </c>
       <c r="L347" s="17"/>
       <c r="M347" s="17"/>
@@ -17413,7 +17413,7 @@
       <c r="Q347" s="17"/>
       <c r="R347" s="18"/>
       <c r="S347" s="19" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
       <c r="T347" s="20" t="s">
         <v>29</v>
@@ -17443,7 +17443,7 @@
         <v>807</v>
       </c>
       <c r="K348" s="17" t="s">
-        <v>894</v>
+        <v>891</v>
       </c>
       <c r="L348" s="17"/>
       <c r="M348" s="17"/>
@@ -17453,7 +17453,7 @@
       <c r="Q348" s="17"/>
       <c r="R348" s="18"/>
       <c r="S348" s="19" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
       <c r="T348" s="20" t="s">
         <v>29</v>
@@ -17483,7 +17483,7 @@
         <v>807</v>
       </c>
       <c r="K349" s="17" t="s">
-        <v>894</v>
+        <v>891</v>
       </c>
       <c r="L349" s="17"/>
       <c r="M349" s="17"/>
@@ -17493,7 +17493,7 @@
       <c r="Q349" s="17"/>
       <c r="R349" s="18"/>
       <c r="S349" s="19" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
       <c r="T349" s="20" t="s">
         <v>29</v>
@@ -17523,7 +17523,7 @@
         <v>807</v>
       </c>
       <c r="K350" s="17" t="s">
-        <v>894</v>
+        <v>891</v>
       </c>
       <c r="L350" s="17"/>
       <c r="M350" s="17"/>
@@ -17533,7 +17533,7 @@
       <c r="Q350" s="17"/>
       <c r="R350" s="18"/>
       <c r="S350" s="19" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
       <c r="T350" s="20" t="s">
         <v>29</v>
@@ -17559,13 +17559,13 @@
         <v>45063</v>
       </c>
       <c r="G351" s="16" t="s">
-        <v>886</v>
+        <v>883</v>
       </c>
       <c r="H351" s="16" t="s">
-        <v>887</v>
+        <v>884</v>
       </c>
       <c r="I351" s="16" t="s">
-        <v>888</v>
+        <v>885</v>
       </c>
       <c r="J351" s="17" t="s">
         <v>467</v>
@@ -17578,7 +17578,7 @@
         <v>467</v>
       </c>
       <c r="N351" s="17" t="s">
-        <v>889</v>
+        <v>886</v>
       </c>
       <c r="O351" s="17" t="s">
         <v>807</v>
@@ -17589,7 +17589,7 @@
       <c r="Q351" s="17"/>
       <c r="R351" s="18"/>
       <c r="S351" s="19" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="T351" s="20" t="s">
         <v>29</v>
@@ -17615,13 +17615,13 @@
         <v>45063</v>
       </c>
       <c r="G352" s="16" t="s">
-        <v>890</v>
+        <v>887</v>
       </c>
       <c r="H352" s="16" t="s">
-        <v>891</v>
+        <v>888</v>
       </c>
       <c r="I352" s="16" t="s">
-        <v>892</v>
+        <v>889</v>
       </c>
       <c r="J352" s="17" t="s">
         <v>467</v>
@@ -17634,7 +17634,7 @@
         <v>467</v>
       </c>
       <c r="N352" s="17" t="s">
-        <v>893</v>
+        <v>890</v>
       </c>
       <c r="O352" s="17" t="s">
         <v>807</v>
@@ -17645,7 +17645,7 @@
       <c r="Q352" s="17"/>
       <c r="R352" s="18"/>
       <c r="S352" s="19" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="T352" s="20" t="s">
         <v>29</v>

</xml_diff>